<commit_message>
Added integration of video
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alvaro/Google Drive/PWScale/Iterative PWScale/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F3519D-323C-EC45-88E2-E4B8FF3B70C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE437E48-E785-7A40-99A0-976742300B4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{3EE04F1E-1415-3B4D-9BE5-D43A373F17F0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="2" xr2:uid="{3EE04F1E-1415-3B4D-9BE5-D43A373F17F0}"/>
   </bookViews>
   <sheets>
     <sheet name="SA" sheetId="3" r:id="rId1"/>
@@ -52,12 +52,6 @@
     <t>Suited for</t>
   </si>
   <si>
-    <t>Very Uncomfortable</t>
-  </si>
-  <si>
-    <t>Very Comfortable</t>
-  </si>
-  <si>
     <t>The sooner we all acquire similar values and ideals the better.</t>
   </si>
   <si>
@@ -845,6 +839,12 @@
   </si>
   <si>
     <t>SA_W_6</t>
+  </si>
+  <si>
+    <t>Strongly Disagree</t>
+  </si>
+  <si>
+    <t>Strongly Agree</t>
   </si>
 </sst>
 </file>
@@ -1204,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B7589F-2305-7A4A-BAC9-2A9F0A317C52}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1234,21 +1234,21 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>268</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1265,13 +1265,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1288,13 +1288,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1311,13 +1311,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1334,13 +1334,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1357,13 +1357,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1389,7 +1389,7 @@
   <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A81"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1413,18 +1413,18 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>268</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1441,10 +1441,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1461,10 +1461,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1481,10 +1481,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1501,10 +1501,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1521,10 +1521,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1541,10 +1541,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1561,10 +1561,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1581,10 +1581,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1601,10 +1601,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1621,10 +1621,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1641,10 +1641,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1661,10 +1661,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1681,10 +1681,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1701,10 +1701,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1721,10 +1721,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1741,10 +1741,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1761,10 +1761,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1781,10 +1781,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1801,10 +1801,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1821,10 +1821,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1841,10 +1841,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1861,10 +1861,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1881,10 +1881,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1901,10 +1901,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1921,10 +1921,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1941,10 +1941,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -1961,10 +1961,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1981,10 +1981,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2001,10 +2001,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2021,10 +2021,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2041,10 +2041,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2061,10 +2061,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2081,10 +2081,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2101,10 +2101,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2121,10 +2121,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2141,10 +2141,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2161,10 +2161,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2181,10 +2181,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2201,10 +2201,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2221,10 +2221,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2241,10 +2241,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2261,10 +2261,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B44" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -2281,10 +2281,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2301,10 +2301,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B46" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -2321,10 +2321,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -2341,10 +2341,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -2361,10 +2361,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B49" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -2381,10 +2381,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B50" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -2401,10 +2401,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B51" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -2421,10 +2421,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -2441,10 +2441,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -2461,10 +2461,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -2481,10 +2481,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -2501,10 +2501,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B56" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -2521,10 +2521,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B57" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -2541,10 +2541,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -2561,10 +2561,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B59" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -2581,10 +2581,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -2601,10 +2601,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B61" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -2621,10 +2621,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B62" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -2641,10 +2641,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B63" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -2661,10 +2661,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B64" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -2681,10 +2681,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B65" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -2701,10 +2701,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B66" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -2721,10 +2721,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B67" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -2741,10 +2741,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B68" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -2761,10 +2761,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B69" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -2781,10 +2781,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B70" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -2801,10 +2801,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B71" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -2821,10 +2821,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B72" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -2841,10 +2841,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B73" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -2861,10 +2861,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B74" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -2881,10 +2881,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B75" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -2901,10 +2901,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B76" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -2921,10 +2921,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B77" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -2941,10 +2941,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B78" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -2961,10 +2961,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B79" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -2981,10 +2981,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B80" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -3001,10 +3001,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B81" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -3029,8 +3029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16618C6F-F7FF-A643-A8B3-B456366D5B94}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3052,18 +3052,18 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>268</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3080,10 +3080,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3120,10 +3120,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3140,10 +3140,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -3160,10 +3160,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3180,10 +3180,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -3200,10 +3200,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3220,10 +3220,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -3240,10 +3240,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -3260,10 +3260,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -3280,10 +3280,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -3300,10 +3300,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -3320,10 +3320,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3340,10 +3340,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -3360,10 +3360,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -3380,10 +3380,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -3400,10 +3400,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -3420,10 +3420,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -3440,10 +3440,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -3460,10 +3460,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3480,10 +3480,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -3500,10 +3500,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3520,10 +3520,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3540,10 +3540,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3560,10 +3560,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3580,10 +3580,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -3600,10 +3600,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -3620,10 +3620,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -3640,10 +3640,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -3660,10 +3660,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3680,10 +3680,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3700,10 +3700,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -3720,10 +3720,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -3740,10 +3740,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -3760,10 +3760,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -3780,10 +3780,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -3800,10 +3800,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -3820,10 +3820,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -3840,10 +3840,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -3860,10 +3860,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B42" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -3880,10 +3880,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -3900,10 +3900,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -3920,10 +3920,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B45" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -3940,10 +3940,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -3960,10 +3960,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B47" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -3980,10 +3980,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B48" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -4000,10 +4000,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B49" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -4020,10 +4020,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B50" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -4040,10 +4040,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -4060,10 +4060,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -4080,10 +4080,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -4100,10 +4100,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -4120,10 +4120,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B55" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -4140,10 +4140,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B56" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -4160,10 +4160,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B57" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -4180,10 +4180,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B58" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -4200,10 +4200,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B59" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -4220,10 +4220,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B60" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -4240,10 +4240,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B61" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -4260,10 +4260,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B62" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -4280,10 +4280,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -4300,10 +4300,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B64" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -4320,10 +4320,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -4340,10 +4340,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B66" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -4360,10 +4360,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B67" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -4380,10 +4380,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B68" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -4400,10 +4400,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B69" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -4420,10 +4420,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B70" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -4440,10 +4440,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B71" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -4460,10 +4460,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B72" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -4480,10 +4480,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B73" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -4500,10 +4500,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B74" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -4520,10 +4520,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -4540,10 +4540,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B76" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -4560,10 +4560,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B77" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -4580,10 +4580,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B78" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -4600,10 +4600,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B79" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -4620,10 +4620,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B80" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -4640,10 +4640,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B81" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C81">
         <v>1</v>

</xml_diff>